<commit_message>
Added test files and more training files
</commit_message>
<xml_diff>
--- a/Audio Files.xlsx
+++ b/Audio Files.xlsx
@@ -8,54 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laza9\OneDrive\Documents\raf\DU Projekat 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469086DA-D750-478C-83A4-003BFDAF97E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EE858F-AD34-485F-831B-04C4741962CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="7">
   <si>
     <t>file</t>
   </si>
   <si>
     <t>text</t>
-  </si>
-  <si>
-    <t>/audio/audio1 (1).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio1 (2).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio1 (3).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio1 (4).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio1 (5).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio2 (1).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio2 (2).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio2 (3).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio2 (4).wav</t>
-  </si>
-  <si>
-    <t>/audio/audio2 (5).wav</t>
   </si>
   <si>
     <t>Tell me the meaning of</t>
@@ -65,6 +35,12 @@
   </si>
   <si>
     <t>What is the meaning of</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -331,10 +307,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -343,7 +319,7 @@
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -351,84 +327,319 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="str">
+        <f>CONCATENATE("/audio/audio1 (", ROW() - 1, ").wav")</f>
+        <v>/audio/audio1 (1).wav</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="str">
+        <f>CONCATENATE("/audio/audio1 (", ROW() - 1, ").wav")</f>
+        <v>/audio/audio1 (2).wav</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="str">
+        <f t="shared" ref="A4:A11" si="0">CONCATENATE("/audio/audio1 (", ROW() - 1, ").wav")</f>
+        <v>/audio/audio1 (3).wav</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/audio/audio1 (4).wav</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/audio/audio1 (5).wav</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/audio/audio1 (6).wav</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/audio/audio1 (7).wav</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/audio/audio1 (8).wav</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/audio/audio1 (9).wav</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/audio/audio1 (10).wav</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="str">
+        <f>CONCATENATE("/audio/audio1 (", ROW() - 1, ").wav")</f>
+        <v>/audio/audio1 (11).wav</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="str">
+        <f>CONCATENATE("/audio/audio1 (", ROW() - 1, ").wav")</f>
+        <v>/audio/audio1 (12).wav</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="str">
+        <f t="shared" ref="A14:A16" si="1">CONCATENATE("/audio/audio1 (", ROW() - 1, ").wav")</f>
+        <v>/audio/audio1 (13).wav</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/audio/audio1 (14).wav</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/audio/audio1 (15).wav</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="str">
+        <f>CONCATENATE("/audio/audio2 (", ROW() - 16, ").wav")</f>
+        <v>/audio/audio2 (1).wav</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="str">
+        <f t="shared" ref="A18:A31" si="2">CONCATENATE("/audio/audio2 (", ROW() - 16, ").wav")</f>
+        <v>/audio/audio2 (2).wav</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (3).wav</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (4).wav</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (5).wav</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (6).wav</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (7).wav</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (8).wav</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (9).wav</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (10).wav</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (11).wav</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (12).wav</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (13).wav</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (14).wav</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>/audio/audio2 (15).wav</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="str">
+        <f>CONCATENATE("/audio/audio3 (", ROW() - 31, ").wav")</f>
+        <v>/audio/audio3 (1).wav</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="str">
+        <f t="shared" ref="A33:A36" si="3">CONCATENATE("/audio/audio3 (", ROW() - 31, ").wav")</f>
+        <v>/audio/audio3 (2).wav</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>/audio/audio3 (3).wav</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>/audio/audio3 (4).wav</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>/audio/audio3 (5).wav</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed reference to blank audio
</commit_message>
<xml_diff>
--- a/Audio Files.xlsx
+++ b/Audio Files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laza9\OneDrive\Documents\raf\DU Projekat 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EE858F-AD34-485F-831B-04C4741962CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2BA55D-F997-4BFE-B54A-8224F6BF8E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
   <si>
     <t>file</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>What is the meaning of</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -309,8 +303,8 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="A32:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -598,49 +592,24 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="str">
-        <f>CONCATENATE("/audio/audio3 (", ROW() - 31, ").wav")</f>
-        <v>/audio/audio3 (1).wav</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="str">
-        <f t="shared" ref="A33:A36" si="3">CONCATENATE("/audio/audio3 (", ROW() - 31, ").wav")</f>
-        <v>/audio/audio3 (2).wav</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>/audio/audio3 (3).wav</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>/audio/audio3 (4).wav</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>/audio/audio3 (5).wav</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>